<commit_message>
updated code and irrigation timing data
</commit_message>
<xml_diff>
--- a/data-raw/irrigation.xlsx
+++ b/data-raw/irrigation.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/biochar_water_conserve/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5AF7E3-7D20-0548-9B47-C33DE172A3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CDD151-65D0-7C42-98CB-2742E703C369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="5920" windowWidth="28040" windowHeight="17440" xr2:uid="{4C42D997-4DFF-DD49-9482-D6C796CD1CF0}"/>
+    <workbookView xWindow="51200" yWindow="22040" windowWidth="23360" windowHeight="14660" xr2:uid="{4C42D997-4DFF-DD49-9482-D6C796CD1CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
   <si>
     <t>DATE</t>
   </si>
@@ -79,7 +79,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -110,11 +110,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,30 +433,31 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
@@ -475,19 +477,19 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>45069</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>0.64236111111111105</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>0.80486111111111114</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="1">
         <f>D2-C2</f>
         <v>0.16250000000000009</v>
       </c>
@@ -508,19 +510,19 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>45078</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>0.51111111111111118</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>0.78125</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <f>D3-C3</f>
         <v>0.27013888888888882</v>
       </c>
@@ -541,21 +543,20 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>45103</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>0.39652777777777781</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>0.66805555555555562</v>
       </c>
-      <c r="E4" s="3">
-        <f t="shared" ref="E4:E19" si="0">D4-C4</f>
-        <v>0.27152777777777781</v>
+      <c r="E4" s="1">
+        <v>0.27152777777777776</v>
       </c>
       <c r="F4">
         <v>225</v>
@@ -574,20 +575,19 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>45124</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>0.33611111111111108</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="3">
         <v>0.6694444444444444</v>
       </c>
-      <c r="E5" s="3">
-        <f t="shared" si="0"/>
+      <c r="E5" s="1">
         <v>0.33333333333333331</v>
       </c>
       <c r="F5">
@@ -607,21 +607,20 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>45143</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>0.3666666666666667</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <v>0.62222222222222223</v>
       </c>
-      <c r="E6" s="3">
-        <f t="shared" si="0"/>
-        <v>0.25555555555555554</v>
+      <c r="E6" s="1">
+        <v>0.25555555555555559</v>
       </c>
       <c r="F6">
         <v>275</v>
@@ -640,41 +639,45 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>45163</v>
+      <c r="A7" s="2">
+        <v>45162</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="C7" s="4">
+        <v>0.57430555555555551</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.76111111111111107</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.18680555555555556</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>225</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>225</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>175450</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>176655</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>60250</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="A8" s="2">
         <v>45183</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="3">
-        <f t="shared" si="0"/>
+      <c r="E8" s="1">
         <v>0</v>
       </c>
       <c r="F8">
@@ -694,14 +697,13 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="A9" s="2">
         <v>45203</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="3">
-        <f t="shared" si="0"/>
+      <c r="E9" s="1">
         <v>0</v>
       </c>
       <c r="F9">
@@ -721,14 +723,13 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="A10" s="2">
         <v>45223</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="3">
-        <f t="shared" si="0"/>
+      <c r="E10" s="1">
         <v>0</v>
       </c>
       <c r="F10">
@@ -748,21 +749,20 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>45070</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>0.3923611111111111</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="3">
         <v>0.55486111111111114</v>
       </c>
-      <c r="E11" s="3">
-        <f t="shared" si="0"/>
-        <v>0.16250000000000003</v>
+      <c r="E11" s="1">
+        <v>0.16250000000000001</v>
       </c>
       <c r="F11">
         <v>575</v>
@@ -781,21 +781,20 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+      <c r="A12" s="2">
         <v>45079</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <v>0.65486111111111112</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="3">
         <v>0.92499999999999993</v>
       </c>
-      <c r="E12" s="3">
-        <f t="shared" si="0"/>
-        <v>0.27013888888888882</v>
+      <c r="E12" s="1">
+        <v>0.27013888888888887</v>
       </c>
       <c r="F12">
         <v>260</v>
@@ -814,21 +813,20 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>45091</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="3">
         <v>0.35069444444444442</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="3">
         <v>0.7284722222222223</v>
       </c>
-      <c r="E13" s="3">
-        <f t="shared" si="0"/>
-        <v>0.37777777777777788</v>
+      <c r="E13" s="1">
+        <v>0.37777777777777777</v>
       </c>
       <c r="F13">
         <v>250</v>
@@ -847,21 +845,20 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+      <c r="A14" s="2">
         <v>45104</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
         <v>0.32847222222222222</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="3">
         <v>0.67638888888888893</v>
       </c>
-      <c r="E14" s="3">
-        <f t="shared" si="0"/>
-        <v>0.34791666666666671</v>
+      <c r="E14" s="1">
+        <v>0.34791666666666665</v>
       </c>
       <c r="F14">
         <v>275</v>
@@ -880,20 +877,19 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+      <c r="A15" s="2">
         <v>45114</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="3">
         <v>0.32361111111111113</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="3">
         <v>0.65694444444444444</v>
       </c>
-      <c r="E15" s="3">
-        <f t="shared" si="0"/>
+      <c r="E15" s="1">
         <v>0.33333333333333331</v>
       </c>
       <c r="F15">
@@ -913,21 +909,20 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+      <c r="A16" s="2">
         <v>45124</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="3">
         <v>0.80486111111111114</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="3">
         <v>0.24513888888888888</v>
       </c>
-      <c r="E16" s="3">
-        <f t="shared" si="0"/>
-        <v>-0.55972222222222223</v>
+      <c r="E16" s="1">
+        <v>0.55972222222222223</v>
       </c>
       <c r="F16">
         <v>225</v>
@@ -946,21 +941,20 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+      <c r="A17" s="2">
         <v>45134</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="3">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="3">
         <v>0.7284722222222223</v>
       </c>
-      <c r="E17" s="3">
-        <f t="shared" si="0"/>
-        <v>0.31180555555555561</v>
+      <c r="E17" s="1">
+        <v>0.31180555555555556</v>
       </c>
       <c r="F17">
         <v>200</v>
@@ -979,21 +973,20 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+      <c r="A18" s="2">
         <v>45143</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="3">
         <v>0.36874999999999997</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="3">
         <v>0.4604166666666667</v>
       </c>
-      <c r="E18" s="3">
-        <f t="shared" si="0"/>
-        <v>9.166666666666673E-2</v>
+      <c r="E18" s="1">
+        <v>9.1666666666666674E-2</v>
       </c>
       <c r="F18">
         <v>250</v>
@@ -1012,21 +1005,20 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+      <c r="A19" s="2">
         <v>45148</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="3">
         <v>0.58124999999999993</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="3">
         <v>0.81736111111111109</v>
       </c>
-      <c r="E19" s="3">
-        <f t="shared" si="0"/>
-        <v>0.23611111111111116</v>
+      <c r="E19" s="1">
+        <v>0.23611111111111113</v>
       </c>
       <c r="F19">
         <v>300</v>
@@ -1044,8 +1036,69 @@
         <v>105700</v>
       </c>
     </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>45162</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.57430555555555551</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.76111111111111107</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.18680555555555556</v>
+      </c>
+      <c r="F20">
+        <v>225</v>
+      </c>
+      <c r="G20">
+        <v>225</v>
+      </c>
+      <c r="H20">
+        <v>175450</v>
+      </c>
+      <c r="I20">
+        <v>176655</v>
+      </c>
+      <c r="J20">
+        <v>60250</v>
+      </c>
+    </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C21" s="1"/>
+      <c r="A21" s="2">
+        <v>45176</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.31805555555555554</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.7631944444444444</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.44513888888888892</v>
+      </c>
+      <c r="F21">
+        <v>240</v>
+      </c>
+      <c r="G21">
+        <v>280</v>
+      </c>
+      <c r="H21">
+        <v>176662</v>
+      </c>
+      <c r="I21">
+        <v>178239</v>
+      </c>
+      <c r="J21">
+        <v>157700</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update to latest irrigation data
</commit_message>
<xml_diff>
--- a/data-raw/irrigation.xlsx
+++ b/data-raw/irrigation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/biochar_water_conserve/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CDD151-65D0-7C42-98CB-2742E703C369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B4E8AE-F10A-1247-9112-5EB6D6F774B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="22040" windowWidth="23360" windowHeight="14660" xr2:uid="{4C42D997-4DFF-DD49-9482-D6C796CD1CF0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="12">
   <si>
     <t>DATE</t>
   </si>
@@ -430,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{810F3BD3-E32C-944A-BCA3-CC03F77368AB}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C22" sqref="C22:J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -672,33 +672,39 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>45183</v>
+        <v>45190</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
+      <c r="C8" s="4">
+        <v>0.37986111111111115</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.67291666666666661</v>
+      </c>
       <c r="E8" s="1">
-        <v>0</v>
+        <v>0.29305555555555557</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>275</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>178252</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>179005</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>75300</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>45203</v>
+        <v>45218</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -1098,6 +1104,54 @@
       </c>
       <c r="J21">
         <v>157700</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>45191</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.30555555555555552</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0.6791666666666667</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.37361111111111112</v>
+      </c>
+      <c r="F22">
+        <v>200</v>
+      </c>
+      <c r="G22">
+        <v>390</v>
+      </c>
+      <c r="H22">
+        <v>179007</v>
+      </c>
+      <c r="I22">
+        <v>180453</v>
+      </c>
+      <c r="J22">
+        <v>144600</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>45205</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>45219</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleanup and addition of averageStrips.R which averages across the data loggers in each strip and plots the results for the west (1 and 2) and east (3 and 4) strips.
</commit_message>
<xml_diff>
--- a/data-raw/irrigation.xlsx
+++ b/data-raw/irrigation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/biochar_water_conserve/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B4E8AE-F10A-1247-9112-5EB6D6F774B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44844B06-3949-394D-8F0B-309412000F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="22040" windowWidth="23360" windowHeight="14660" xr2:uid="{4C42D997-4DFF-DD49-9482-D6C796CD1CF0}"/>
+    <workbookView xWindow="52280" yWindow="22260" windowWidth="23360" windowHeight="14660" xr2:uid="{4C42D997-4DFF-DD49-9482-D6C796CD1CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
   <si>
     <t>DATE</t>
   </si>
@@ -112,10 +112,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,728 +430,714 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{810F3BD3-E32C-944A-BCA3-CC03F77368AB}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:J22"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="4" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" style="4"/>
+    <col min="8" max="8" width="14.83203125" style="4" customWidth="1"/>
+    <col min="9" max="10" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>45069</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>0.64236111111111105</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>0.80486111111111114</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="4">
         <f>D2-C2</f>
         <v>0.16250000000000009</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="4">
         <v>550</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="4">
         <v>550</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="4">
         <v>160574</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="4">
         <v>162024</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="4">
         <v>145000</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>45078</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>0.51111111111111118</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>0.78125</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="4">
         <f>D3-C3</f>
         <v>0.27013888888888882</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="4">
         <v>200</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="4">
         <v>290</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="4">
         <v>163494</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="4">
         <v>164167</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="4">
         <v>67300</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>45103</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>0.39652777777777781</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>0.66805555555555562</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <v>0.27152777777777776</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="4">
         <v>225</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <v>225</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <v>166136</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="4">
         <v>167030</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="4">
         <v>89400</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>45124</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>0.33611111111111108</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>0.6694444444444444</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="4">
         <v>295</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="4">
         <v>250</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="4">
         <v>169684</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="4">
         <v>170893</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="4">
         <v>120900</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>45143</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>0.3666666666666667</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>0.62222222222222223</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="4">
         <v>0.25555555555555559</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="4">
         <v>275</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="4">
         <v>250</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="4">
         <v>173025</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="4">
         <v>174376</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="4">
         <v>98500</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>45162</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>0.57430555555555551</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>0.76111111111111107</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="4">
         <v>0.18680555555555556</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="4">
         <v>225</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="4">
         <v>225</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="4">
         <v>175450</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="4">
         <v>176655</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="4">
         <v>60250</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>45190</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>0.37986111111111115</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>0.67291666666666661</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="4">
         <v>0.29305555555555557</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="4">
         <v>275</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="4">
         <v>150</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="4">
         <v>178252</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="4">
         <v>179005</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="4">
         <v>75300</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>45218</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>45223</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>45070</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>0.3923611111111111</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>0.55486111111111114</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="4">
         <v>0.16250000000000001</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="4">
         <v>575</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="4">
         <v>700</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="4">
         <v>162026</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="4">
         <v>163492</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="4">
         <v>146600</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>45079</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>0.65486111111111112</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>0.92499999999999993</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="4">
         <v>0.27013888888888887</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="4">
         <v>260</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="4">
         <v>250</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="4">
         <v>164171</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="4">
         <v>164846</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="4">
         <v>67500</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>45091</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>0.35069444444444442</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>0.7284722222222223</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="4">
         <v>0.37777777777777777</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="4">
         <v>250</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="4">
         <v>250</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="4">
         <v>164847</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="4">
         <v>166129</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="4">
         <v>128200</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>45104</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>0.32847222222222222</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>0.67638888888888893</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="4">
         <v>0.34791666666666665</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="4">
         <v>275</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="4">
         <v>275</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="4">
         <v>167039</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="4">
         <v>168396</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="4">
         <v>135700</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>45114</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>0.32361111111111113</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>0.65694444444444444</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="4">
         <v>300</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="4">
         <v>250</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="4">
         <v>168398</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="4">
         <v>169683</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="4">
         <v>128500</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>45124</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>0.80486111111111114</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>0.24513888888888888</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="4">
         <v>0.55972222222222223</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="4">
         <v>225</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="4">
         <v>290</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="4">
         <v>170904</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="4">
         <v>172513</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="4">
         <v>160900</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>45134</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>0.7284722222222223</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="4">
         <v>0.31180555555555556</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="4">
         <v>200</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="4">
         <v>90</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="4">
         <v>172515</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="4">
         <v>173019</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="4">
         <v>50400</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>45143</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>0.36874999999999997</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>0.4604166666666667</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="4">
         <v>9.1666666666666674E-2</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="4">
         <v>250</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="4">
         <v>175</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="4">
         <v>173262</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="4">
         <v>173628</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="4">
         <v>36600</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>45148</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>0.58124999999999993</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>0.81736111111111109</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="4">
         <v>0.23611111111111113</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="4">
         <v>300</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="4">
         <v>325</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="4">
         <v>174384</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="4">
         <v>175441</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="4">
         <v>105700</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>45162</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>0.57430555555555551</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <v>0.76111111111111107</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="4">
         <v>0.18680555555555556</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="4">
         <v>225</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="4">
         <v>225</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="4">
         <v>175450</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="4">
         <v>176655</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="4">
         <v>60250</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>45176</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>0.31805555555555554</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>0.7631944444444444</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="4">
         <v>0.44513888888888892</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="4">
         <v>240</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="4">
         <v>280</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="4">
         <v>176662</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="4">
         <v>178239</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="4">
         <v>157700</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>45191</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>0.30555555555555552</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <v>0.6791666666666667</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="4">
         <v>0.37361111111111112</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="4">
         <v>200</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="4">
         <v>390</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="4">
         <v>179007</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="4">
         <v>180453</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="4">
         <v>144600</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
-        <v>45205</v>
-      </c>
-      <c r="B23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
-        <v>45219</v>
-      </c>
-      <c r="B24" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleanup of 4 files.
</commit_message>
<xml_diff>
--- a/data-raw/irrigation.xlsx
+++ b/data-raw/irrigation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/biochar_water_conserve/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44844B06-3949-394D-8F0B-309412000F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8918CA-A91F-EB4B-A387-0CBB9D67C3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52280" yWindow="22260" windowWidth="23360" windowHeight="14660" xr2:uid="{4C42D997-4DFF-DD49-9482-D6C796CD1CF0}"/>
+    <workbookView xWindow="6900" yWindow="2620" windowWidth="23360" windowHeight="14660" xr2:uid="{4C42D997-4DFF-DD49-9482-D6C796CD1CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
   <si>
     <t>DATE</t>
   </si>
@@ -430,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{810F3BD3-E32C-944A-BCA3-CC03F77368AB}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -441,7 +441,8 @@
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11.5" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="4" customWidth="1"/>
-    <col min="6" max="7" width="10.83203125" style="4"/>
+    <col min="6" max="6" width="18" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="4"/>
     <col min="8" max="8" width="14.83203125" style="4" customWidth="1"/>
     <col min="9" max="10" width="10.83203125" style="4"/>
   </cols>
@@ -706,437 +707,385 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>45218</v>
+        <v>45070</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.55486111111111114</v>
       </c>
       <c r="E9" s="4">
-        <v>0</v>
+        <v>0.16250000000000001</v>
       </c>
       <c r="F9" s="4">
-        <v>0</v>
+        <v>575</v>
       </c>
       <c r="G9" s="4">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="H9" s="4">
-        <v>0</v>
+        <v>162026</v>
       </c>
       <c r="I9" s="4">
-        <v>0</v>
+        <v>163492</v>
       </c>
       <c r="J9" s="4">
-        <v>0</v>
+        <v>146600</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>45223</v>
+        <v>45079</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.65486111111111112</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.92499999999999993</v>
       </c>
       <c r="E10" s="4">
-        <v>0</v>
+        <v>0.27013888888888887</v>
       </c>
       <c r="F10" s="4">
-        <v>0</v>
+        <v>260</v>
       </c>
       <c r="G10" s="4">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="H10" s="4">
-        <v>0</v>
+        <v>164171</v>
       </c>
       <c r="I10" s="4">
-        <v>0</v>
+        <v>164846</v>
       </c>
       <c r="J10" s="4">
-        <v>0</v>
+        <v>67500</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>45070</v>
+        <v>45091</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="2">
-        <v>0.3923611111111111</v>
+        <v>0.35069444444444442</v>
       </c>
       <c r="D11" s="2">
-        <v>0.55486111111111114</v>
+        <v>0.7284722222222223</v>
       </c>
       <c r="E11" s="4">
-        <v>0.16250000000000001</v>
+        <v>0.37777777777777777</v>
       </c>
       <c r="F11" s="4">
-        <v>575</v>
+        <v>250</v>
       </c>
       <c r="G11" s="4">
-        <v>700</v>
+        <v>250</v>
       </c>
       <c r="H11" s="4">
-        <v>162026</v>
+        <v>164847</v>
       </c>
       <c r="I11" s="4">
-        <v>163492</v>
+        <v>166129</v>
       </c>
       <c r="J11" s="4">
-        <v>146600</v>
+        <v>128200</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>45079</v>
+        <v>45104</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="2">
-        <v>0.65486111111111112</v>
+        <v>0.32847222222222222</v>
       </c>
       <c r="D12" s="2">
-        <v>0.92499999999999993</v>
+        <v>0.67638888888888893</v>
       </c>
       <c r="E12" s="4">
-        <v>0.27013888888888887</v>
+        <v>0.34791666666666665</v>
       </c>
       <c r="F12" s="4">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="G12" s="4">
-        <v>250</v>
+        <v>275</v>
       </c>
       <c r="H12" s="4">
-        <v>164171</v>
+        <v>167039</v>
       </c>
       <c r="I12" s="4">
-        <v>164846</v>
+        <v>168396</v>
       </c>
       <c r="J12" s="4">
-        <v>67500</v>
+        <v>135700</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>45091</v>
+        <v>45114</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="2">
-        <v>0.35069444444444442</v>
+        <v>0.32361111111111113</v>
       </c>
       <c r="D13" s="2">
-        <v>0.7284722222222223</v>
+        <v>0.65694444444444444</v>
       </c>
       <c r="E13" s="4">
-        <v>0.37777777777777777</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F13" s="4">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="G13" s="4">
         <v>250</v>
       </c>
       <c r="H13" s="4">
-        <v>164847</v>
+        <v>168398</v>
       </c>
       <c r="I13" s="4">
-        <v>166129</v>
+        <v>169683</v>
       </c>
       <c r="J13" s="4">
-        <v>128200</v>
+        <v>128500</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>45104</v>
+        <v>45124</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="2">
-        <v>0.32847222222222222</v>
+        <v>0.80486111111111114</v>
       </c>
       <c r="D14" s="2">
-        <v>0.67638888888888893</v>
+        <v>0.24513888888888888</v>
       </c>
       <c r="E14" s="4">
-        <v>0.34791666666666665</v>
+        <v>0.55972222222222223</v>
       </c>
       <c r="F14" s="4">
-        <v>275</v>
+        <v>225</v>
       </c>
       <c r="G14" s="4">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="H14" s="4">
-        <v>167039</v>
+        <v>170904</v>
       </c>
       <c r="I14" s="4">
-        <v>168396</v>
+        <v>172513</v>
       </c>
       <c r="J14" s="4">
-        <v>135700</v>
+        <v>160900</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>45114</v>
+        <v>45134</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="2">
-        <v>0.32361111111111113</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="D15" s="2">
-        <v>0.65694444444444444</v>
+        <v>0.7284722222222223</v>
       </c>
       <c r="E15" s="4">
-        <v>0.33333333333333331</v>
+        <v>0.31180555555555556</v>
       </c>
       <c r="F15" s="4">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="G15" s="4">
-        <v>250</v>
+        <v>90</v>
       </c>
       <c r="H15" s="4">
-        <v>168398</v>
+        <v>172515</v>
       </c>
       <c r="I15" s="4">
-        <v>169683</v>
+        <v>173019</v>
       </c>
       <c r="J15" s="4">
-        <v>128500</v>
+        <v>50400</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>45124</v>
+        <v>45143</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="2">
-        <v>0.80486111111111114</v>
+        <v>0.36874999999999997</v>
       </c>
       <c r="D16" s="2">
-        <v>0.24513888888888888</v>
+        <v>0.4604166666666667</v>
       </c>
       <c r="E16" s="4">
-        <v>0.55972222222222223</v>
+        <v>9.1666666666666674E-2</v>
       </c>
       <c r="F16" s="4">
-        <v>225</v>
+        <v>250</v>
       </c>
       <c r="G16" s="4">
-        <v>290</v>
+        <v>175</v>
       </c>
       <c r="H16" s="4">
-        <v>170904</v>
+        <v>173262</v>
       </c>
       <c r="I16" s="4">
-        <v>172513</v>
+        <v>173628</v>
       </c>
       <c r="J16" s="4">
-        <v>160900</v>
+        <v>36600</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>45134</v>
+        <v>45148</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="2">
-        <v>0.41666666666666669</v>
+        <v>0.58124999999999993</v>
       </c>
       <c r="D17" s="2">
-        <v>0.7284722222222223</v>
+        <v>0.81736111111111109</v>
       </c>
       <c r="E17" s="4">
-        <v>0.31180555555555556</v>
+        <v>0.23611111111111113</v>
       </c>
       <c r="F17" s="4">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="G17" s="4">
-        <v>90</v>
+        <v>325</v>
       </c>
       <c r="H17" s="4">
-        <v>172515</v>
+        <v>174384</v>
       </c>
       <c r="I17" s="4">
-        <v>173019</v>
+        <v>175441</v>
       </c>
       <c r="J17" s="4">
-        <v>50400</v>
+        <v>105700</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>45143</v>
+        <v>45162</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="2">
-        <v>0.36874999999999997</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.4604166666666667</v>
+      <c r="C18" s="3">
+        <v>0.57430555555555551</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.76111111111111107</v>
       </c>
       <c r="E18" s="4">
-        <v>9.1666666666666674E-2</v>
+        <v>0.18680555555555556</v>
       </c>
       <c r="F18" s="4">
-        <v>250</v>
+        <v>225</v>
       </c>
       <c r="G18" s="4">
-        <v>175</v>
+        <v>225</v>
       </c>
       <c r="H18" s="4">
-        <v>173262</v>
+        <v>175450</v>
       </c>
       <c r="I18" s="4">
-        <v>173628</v>
+        <v>176655</v>
       </c>
       <c r="J18" s="4">
-        <v>36600</v>
+        <v>60250</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>45148</v>
+        <v>45176</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="2">
-        <v>0.58124999999999993</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0.81736111111111109</v>
+      <c r="C19" s="3">
+        <v>0.31805555555555554</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.7631944444444444</v>
       </c>
       <c r="E19" s="4">
-        <v>0.23611111111111113</v>
+        <v>0.44513888888888892</v>
       </c>
       <c r="F19" s="4">
-        <v>300</v>
+        <v>240</v>
       </c>
       <c r="G19" s="4">
-        <v>325</v>
+        <v>280</v>
       </c>
       <c r="H19" s="4">
-        <v>174384</v>
+        <v>176662</v>
       </c>
       <c r="I19" s="4">
-        <v>175441</v>
+        <v>178239</v>
       </c>
       <c r="J19" s="4">
-        <v>105700</v>
+        <v>157700</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>45162</v>
+        <v>45191</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="3">
-        <v>0.57430555555555551</v>
+        <v>0.30555555555555552</v>
       </c>
       <c r="D20" s="3">
-        <v>0.76111111111111107</v>
+        <v>0.6791666666666667</v>
       </c>
       <c r="E20" s="4">
-        <v>0.18680555555555556</v>
+        <v>0.37361111111111112</v>
       </c>
       <c r="F20" s="4">
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="G20" s="4">
-        <v>225</v>
+        <v>390</v>
       </c>
       <c r="H20" s="4">
-        <v>175450</v>
+        <v>179007</v>
       </c>
       <c r="I20" s="4">
-        <v>176655</v>
+        <v>180453</v>
       </c>
       <c r="J20" s="4">
-        <v>60250</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>45176</v>
-      </c>
-      <c r="B21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="3">
-        <v>0.31805555555555554</v>
-      </c>
-      <c r="D21" s="3">
-        <v>0.7631944444444444</v>
-      </c>
-      <c r="E21" s="4">
-        <v>0.44513888888888892</v>
-      </c>
-      <c r="F21" s="4">
-        <v>240</v>
-      </c>
-      <c r="G21" s="4">
-        <v>280</v>
-      </c>
-      <c r="H21" s="4">
-        <v>176662</v>
-      </c>
-      <c r="I21" s="4">
-        <v>178239</v>
-      </c>
-      <c r="J21" s="4">
-        <v>157700</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>45191</v>
-      </c>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="3">
-        <v>0.30555555555555552</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0.6791666666666667</v>
-      </c>
-      <c r="E22" s="4">
-        <v>0.37361111111111112</v>
-      </c>
-      <c r="F22" s="4">
-        <v>200</v>
-      </c>
-      <c r="G22" s="4">
-        <v>390</v>
-      </c>
-      <c r="H22" s="4">
-        <v>179007</v>
-      </c>
-      <c r="I22" s="4">
-        <v>180453</v>
-      </c>
-      <c r="J22" s="4">
         <v>144600</v>
       </c>
     </row>

</xml_diff>